<commit_message>
Completed paper and included slides pdf and other documents
</commit_message>
<xml_diff>
--- a/results/graph-book.xlsx
+++ b/results/graph-book.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usu-my.sharepoint.com/personal/a02039272_aggies_usu_edu/Documents/Documents and Files/School/Graduate/Fall 2022/ReinforcementLearning/FinalProject/results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usu-my.sharepoint.com/personal/a02039272_aggies_usu_edu/Documents/Documents and Files/School/Graduate/Fall 2022/ReinforcementLearning/FinalProject/starting-code/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="116" documentId="8_{5251209B-056C-44C5-B31D-7B62854AC758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9BAFE32F-B4DE-4C6A-BFAF-09E744B9BCB2}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E24FF2D8-06DF-4977-8F45-5524B0C9418C}"/>
+    <workbookView xWindow="-18105" yWindow="-210" windowWidth="18210" windowHeight="11295" xr2:uid="{E24FF2D8-06DF-4977-8F45-5524B0C9418C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>